<commit_message>
finished draft IPTDS recommendations
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230802.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230802.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E563379-C067-4CE5-98BD-3B9C1C1C7094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453F1D68-1AE7-4685-9FFA-80BF2EAD9327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46980" yWindow="-2385" windowWidth="33420" windowHeight="21150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47595" yWindow="-2385" windowWidth="32805" windowHeight="21150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -2925,7 +2925,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2968,12 +2968,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3083,7 +3077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3153,50 +3147,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -15594,24 +15550,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:L27">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M27">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Consider removing IPTDS from Biomark O&amp;M (if any); keep other monitoring method"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Include necessary population-scale IPTDS in Biomark O&amp;M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Population is a candidate for IPTDS in Biomark O&amp;M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"Keep or consider a low-precision method"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15630,7 +15586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B48E5-B2D0-4B19-967E-72BE4D4B4F25}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -15865,7 +15821,7 @@
       <c r="L5" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="M5" s="17" t="s">
         <v>797</v>
       </c>
       <c r="N5" s="16" t="s">
@@ -17590,21 +17546,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:M44">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N44">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Include necessary population-scale IPTDS in Biomark O&amp;M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Consider removing IPTDS from Biomark O&amp;M (if any); keep other monitoring method"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Keep IPTDS or consider a low-precision method"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>